<commit_message>
Update Alpha V0.4 Test
Levels:
 -Optimized method for level generation. Generates buildings by floors instead piece by piece
 -Door now sets inside and outside playlines automatically

PlayerController:
-Door detection by layer

Utilities:
-Added a random enum value method
</commit_message>
<xml_diff>
--- a/RoadMap.xlsx
+++ b/RoadMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UNITY\Zcavenger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3586C1-9401-4A0F-81F8-E3A1ECA6B44E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBB54BA-CF73-4A67-AAE6-52988D02CBBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -275,8 +275,9 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Pflores:
-Head,Torso,Leg</t>
+          <t xml:space="preserve">Pflores:
+Head,Torso,Leg,backpack
+</t>
         </r>
       </text>
     </comment>
@@ -311,30 +312,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="F41" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Pflores:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B42" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
@@ -356,58 +333,11 @@
           </rPr>
           <t xml:space="preserve">
 Grenade ok
-Molovot Cocktail ok
-Rock</t>
+Molovot Cocktail ok</t>
         </r>
       </text>
     </comment>
-    <comment ref="F46" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Pflores:
-Head,Torso,Leg</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B47" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Pflores:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Grab Item
-Use Bandage ok
-Eat Food ok
-Drink Water ok
-Throw objects:
- Grenade ok
- Molotov ok
- Rock ok </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F47" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+    <comment ref="D46" authorId="0" shapeId="0" xr:uid="{A4FEDE02-96DA-485A-A623-E4B7289465E0}">
       <text>
         <r>
           <rPr>
@@ -428,32 +358,6 @@
           </rPr>
           <t xml:space="preserve">
 </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B48" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Usuario de Windows:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Grenade ok
-Molovot Cocktail ok
-Rock</t>
         </r>
       </text>
     </comment>
@@ -496,7 +400,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="328">
   <si>
     <t>Platforms:</t>
   </si>
@@ -1245,9 +1149,6 @@
     <t>Performance: LOD Groups</t>
   </si>
   <si>
-    <t>Levels: Hospital level design</t>
-  </si>
-  <si>
     <t>AI: Player detection by sounds</t>
   </si>
   <si>
@@ -1427,9 +1328,6 @@
     <t>Slow Time</t>
   </si>
   <si>
-    <t>UI: Level Map</t>
-  </si>
-  <si>
     <t>When climbing a ladder player is not aligned with the ladder x-axis</t>
   </si>
   <si>
@@ -1488,9 +1386,6 @@
   </si>
   <si>
     <t>ALPHA V0.5</t>
-  </si>
-  <si>
-    <t>Levels: City</t>
   </si>
   <si>
     <t>Enemy Spawn Manager</t>
@@ -1501,6 +1396,12 @@
   <si>
     <t xml:space="preserve">Levels: Procedural level generation
 </t>
+  </si>
+  <si>
+    <t>Levels: Hospital building design</t>
+  </si>
+  <si>
+    <t>Levels: Demo level</t>
   </si>
 </sst>
 </file>
@@ -1992,7 +1893,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2178,6 +2079,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2485,8 +2389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2612,7 +2516,7 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="19" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="19" t="s">
@@ -2850,7 +2754,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B30" s="13" t="s">
         <v>7</v>
@@ -2877,7 +2781,7 @@
         <v>202</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="F31" s="41" t="s">
         <v>232</v>
@@ -2891,7 +2795,7 @@
     </row>
     <row r="32" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B32" s="41" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="D32" s="41" t="s">
         <v>230</v>
@@ -2967,7 +2871,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B39" s="13" t="s">
         <v>7</v>
@@ -2991,62 +2895,50 @@
     </row>
     <row r="40" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="19" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D40" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="F40" s="62" t="s">
+        <v>270</v>
+      </c>
+      <c r="H40" s="20" t="s">
+        <v>325</v>
+      </c>
+      <c r="J40" s="4"/>
+    </row>
+    <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B41" s="41" t="s">
         <v>246</v>
       </c>
-      <c r="F40" s="43" t="s">
-        <v>271</v>
-      </c>
-      <c r="H40" s="43" t="s">
-        <v>292</v>
-      </c>
-      <c r="J40" s="20" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="120" x14ac:dyDescent="0.25">
-      <c r="B41" s="41" t="s">
+      <c r="D41" s="41" t="s">
+        <v>326</v>
+      </c>
+      <c r="F41" s="64"/>
+      <c r="H41" s="64"/>
+      <c r="J41" s="64"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="41" t="s">
         <v>247</v>
       </c>
-      <c r="D41" s="62" t="s">
-        <v>245</v>
-      </c>
-      <c r="F41" s="43" t="s">
-        <v>291</v>
-      </c>
-      <c r="H41" s="43" t="s">
-        <v>293</v>
-      </c>
-      <c r="J41" s="43" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="62" t="s">
-        <v>248</v>
-      </c>
-      <c r="D42" s="62" t="s">
-        <v>322</v>
+      <c r="D42" s="41" t="s">
+        <v>320</v>
       </c>
       <c r="F42" s="55"/>
-      <c r="H42" s="43" t="s">
-        <v>294</v>
-      </c>
+      <c r="H42" s="64"/>
       <c r="J42" s="55"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B43" s="41" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D43" s="41" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F43" s="55"/>
-      <c r="H43" s="43" t="s">
-        <v>308</v>
-      </c>
+      <c r="H43" s="64"/>
       <c r="J43" s="55"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -3058,7 +2950,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B45" s="13" t="s">
         <v>7</v>
@@ -3080,29 +2972,39 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="F46" s="63"/>
-      <c r="H46" s="63"/>
+    <row r="46" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="B46" s="43" t="s">
+        <v>291</v>
+      </c>
+      <c r="D46" s="43" t="s">
+        <v>290</v>
+      </c>
+      <c r="F46" s="43" t="s">
+        <v>292</v>
+      </c>
+      <c r="H46" s="43" t="s">
+        <v>306</v>
+      </c>
       <c r="J46" s="4"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="63"/>
+      <c r="B47" s="64"/>
       <c r="D47" s="63"/>
-      <c r="F47" s="63"/>
+      <c r="F47" s="43" t="s">
+        <v>293</v>
+      </c>
       <c r="H47" s="63"/>
       <c r="J47" s="63"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B48" s="63"/>
+      <c r="B48" s="64"/>
       <c r="D48" s="63"/>
       <c r="F48" s="63"/>
       <c r="H48" s="63"/>
       <c r="J48" s="63"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B49" s="63"/>
+      <c r="B49" s="64"/>
       <c r="D49" s="63"/>
       <c r="F49" s="63"/>
       <c r="H49" s="63"/>
@@ -3404,7 +3306,7 @@
       </c>
       <c r="E10" s="39"/>
       <c r="F10" s="39" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G10" s="39" t="s">
         <v>190</v>
@@ -3421,20 +3323,20 @@
         <v>11</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C11" s="32" t="s">
         <v>147</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E11" s="39"/>
       <c r="F11" s="39" t="s">
+        <v>253</v>
+      </c>
+      <c r="G11" s="39" t="s">
         <v>254</v>
-      </c>
-      <c r="G11" s="39" t="s">
-        <v>255</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="22"/>
@@ -3448,20 +3350,20 @@
         <v>11</v>
       </c>
       <c r="B12" s="58" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C12" s="32" t="s">
         <v>147</v>
       </c>
       <c r="D12" s="60" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E12" s="61"/>
       <c r="F12" s="61" t="s">
+        <v>268</v>
+      </c>
+      <c r="G12" s="61" t="s">
         <v>269</v>
-      </c>
-      <c r="G12" s="61" t="s">
-        <v>270</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="56"/>
@@ -3475,20 +3377,20 @@
         <v>11</v>
       </c>
       <c r="B13" s="58" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C13" s="59" t="s">
         <v>147</v>
       </c>
       <c r="D13" s="60" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E13" s="61"/>
       <c r="F13" s="61" t="s">
+        <v>257</v>
+      </c>
+      <c r="G13" s="61" t="s">
         <v>258</v>
-      </c>
-      <c r="G13" s="61" t="s">
-        <v>259</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="22"/>
@@ -3502,20 +3404,20 @@
         <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C14" s="33" t="s">
         <v>146</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="G14" s="39" t="s">
         <v>262</v>
-      </c>
-      <c r="G14" s="39" t="s">
-        <v>263</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="56"/>
@@ -3535,14 +3437,14 @@
         <v>146</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="G15" s="39" t="s">
         <v>265</v>
-      </c>
-      <c r="G15" s="39" t="s">
-        <v>266</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="56"/>
@@ -3562,14 +3464,14 @@
         <v>146</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="G16" s="39" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="56"/>
@@ -3611,10 +3513,10 @@
       <c r="M18" s="7"/>
     </row>
     <row r="19" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="64"/>
-      <c r="B19" s="64"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="64"/>
+      <c r="A19" s="65"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
@@ -3626,10 +3528,10 @@
       <c r="M19" s="7"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="64"/>
-      <c r="B20" s="64"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
+      <c r="A20" s="65"/>
+      <c r="B20" s="65"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="65"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
@@ -3641,10 +3543,10 @@
       <c r="M20" s="7"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="64"/>
-      <c r="B21" s="64"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="64"/>
+      <c r="A21" s="65"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="65"/>
       <c r="E21" s="25"/>
       <c r="F21" s="25"/>
       <c r="G21" s="25"/>
@@ -3656,20 +3558,20 @@
       <c r="M21" s="7"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="64"/>
-      <c r="B22" s="64"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
+      <c r="A22" s="65"/>
+      <c r="B22" s="65"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="64"/>
-      <c r="B23" s="64"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
+      <c r="A23" s="65"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
@@ -3874,10 +3776,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="66"/>
+      <c r="C2" s="67"/>
     </row>
     <row r="4" spans="2:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
@@ -4942,10 +4844,10 @@
         <v>6002</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>74</v>
@@ -5031,7 +4933,7 @@
         <v>6005</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D43" s="55"/>
       <c r="E43" s="55">
@@ -5093,7 +4995,7 @@
         <v>60</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="55"/>
@@ -5122,7 +5024,7 @@
         <v>169</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E47" s="5"/>
       <c r="F47" s="55"/>
@@ -5148,10 +5050,10 @@
         <v>7003</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48" s="55"/>
@@ -5180,7 +5082,7 @@
         <v>67</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="55"/>
@@ -5213,7 +5115,7 @@
         <v>68</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E50" s="5"/>
       <c r="F50" s="55"/>
@@ -5243,10 +5145,10 @@
         <v>7006</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D51" s="55" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E51" s="55"/>
       <c r="F51" s="55"/>
@@ -5266,10 +5168,10 @@
         <v>7007</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D52" s="55" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E52" s="55"/>
       <c r="F52" s="55"/>
@@ -5289,10 +5191,10 @@
         <v>7008</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D53" s="55" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E53" s="55"/>
       <c r="F53" s="55"/>
@@ -5797,7 +5699,7 @@
         <v>110001</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D75" s="44"/>
       <c r="E75" s="44"/>
@@ -5822,7 +5724,7 @@
         <v>110002</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D76" s="44"/>
       <c r="E76" s="44"/>
@@ -5847,7 +5749,7 @@
         <v>110003</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D77" s="55"/>
       <c r="E77" s="55"/>
@@ -5868,7 +5770,7 @@
         <v>110004</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D78" s="55"/>
       <c r="E78" s="55"/>
@@ -5889,7 +5791,7 @@
         <v>110005</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D79" s="55"/>
       <c r="E79" s="55"/>
@@ -5910,7 +5812,7 @@
         <v>110006</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D80" s="55"/>
       <c r="E80" s="55"/>
@@ -5950,7 +5852,7 @@
     <row r="82" spans="2:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="14"/>
       <c r="C82" s="14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D82" s="55"/>
       <c r="E82" s="55"/>
@@ -5971,7 +5873,7 @@
         <v>120001</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D83" s="55"/>
       <c r="E83" s="55"/>
@@ -5996,7 +5898,7 @@
         <v>120002</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D84" s="55"/>
       <c r="E84" s="55"/>
@@ -6021,7 +5923,7 @@
         <v>120003</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D85" s="55"/>
       <c r="E85" s="55"/>
@@ -6042,7 +5944,7 @@
         <v>120004</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D86" s="55"/>
       <c r="E86" s="55"/>
@@ -6063,7 +5965,7 @@
         <v>120005</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D87" s="55"/>
       <c r="E87" s="55"/>
@@ -6088,7 +5990,7 @@
         <v>120006</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D88" s="55"/>
       <c r="E88" s="55"/>
@@ -6109,7 +6011,7 @@
         <v>120007</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D89" s="55"/>
       <c r="E89" s="55"/>
@@ -6149,7 +6051,7 @@
     <row r="91" spans="2:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="14"/>
       <c r="C91" s="14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D91" s="55"/>
       <c r="E91" s="55"/>
@@ -6170,7 +6072,7 @@
         <v>130001</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D92" s="55"/>
       <c r="E92" s="55"/>
@@ -6195,7 +6097,7 @@
         <v>130002</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D93" s="55"/>
       <c r="E93" s="55"/>
@@ -6220,7 +6122,7 @@
         <v>130003</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D94" s="55"/>
       <c r="E94" s="55"/>
@@ -6245,7 +6147,7 @@
         <v>130004</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D95" s="55"/>
       <c r="E95" s="55"/>
@@ -6315,7 +6217,7 @@
     <row r="99" spans="2:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" s="14"/>
       <c r="C99" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D99" s="55"/>
       <c r="E99" s="55"/>
@@ -6336,7 +6238,7 @@
         <v>140001</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D100" s="55"/>
       <c r="E100" s="55"/>
@@ -6361,7 +6263,7 @@
         <v>140002</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D101" s="55"/>
       <c r="E101" s="55"/>
@@ -6386,7 +6288,7 @@
         <v>140003</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D102" s="55"/>
       <c r="E102" s="55"/>
@@ -6411,7 +6313,7 @@
         <v>140004</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D103" s="55"/>
       <c r="E103" s="55"/>
@@ -6503,10 +6405,10 @@
   <sheetData>
     <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="68" t="s">
         <v>228</v>
       </c>
-      <c r="C2" s="68"/>
+      <c r="C2" s="69"/>
     </row>
     <row r="4" spans="2:15" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">

</xml_diff>